<commit_message>
Ocean accounts to RDF/TTL
</commit_message>
<xml_diff>
--- a/crosswalks/Coastal-IUCNGET/Coastal-IUCNGET.xlsx
+++ b/crosswalks/Coastal-IUCNGET/Coastal-IUCNGET.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ecosystem-typology\crosswalks\Coastal-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C66DFC9-CFAB-4056-9063-5B2418BD981C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34441608-E21C-461C-A627-28E2A884AFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="945" yWindow="9315" windowWidth="34230" windowHeight="10815" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>